<commit_message>
Corrected the generated file extension
</commit_message>
<xml_diff>
--- a/ResxFileFromExcel/SampleInput.xlsx
+++ b/ResxFileFromExcel/SampleInput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ResxFileFromExcel\ResxFileFromExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46E8A55-0F11-41F9-AF78-B0B2F5CFEBB9}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E4504A4-3F77-4766-BC1F-6F2503125C95}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" xr2:uid="{68ABEB2B-1EC0-495F-B6CD-C870869A9683}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="1216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="1214">
   <si>
     <t>This account has been locked out, please try again later</t>
   </si>
@@ -4517,13 +4517,7 @@
     <t>Skicka gratis i-app-meddelanden till familj och vänner om de också har Talk Home-appen.</t>
   </si>
   <si>
-    <t>Du kan även skicka standard-SMS till icke-Talk Home- app-kunder genom att följa följande steg:</t>
-  </si>
-  <si>
     <t>1. Svep till och välj “Meddelande”-ikonen</t>
-  </si>
-  <si>
-    <t>2. Välj plus-ikonen i det övre högra hörnet för att starta ett nytt meddelande</t>
   </si>
   <si>
     <t>3. Skriv in mobiltelefonnumret som du skulle vilja SMS:a till eller välj den gröna plus-knappen för att lägga till någon från din kontaktlista</t>
@@ -5105,8 +5099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1E42DC8-636C-4C44-9197-A5F0246B85D6}">
   <dimension ref="A1:K120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C120" sqref="C120"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7052,7 +7046,7 @@
       <c r="A56" s="10" t="s">
         <v>1054</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="1" t="s">
         <v>1158</v>
       </c>
       <c r="C56" t="s">
@@ -7157,7 +7151,7 @@
       <c r="A59" s="10" t="s">
         <v>1057</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="1" t="s">
         <v>1161</v>
       </c>
       <c r="C59" t="s">
@@ -7573,7 +7567,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="10" t="s">
         <v>1069</v>
       </c>
@@ -7612,8 +7606,8 @@
       <c r="A72" s="10" t="s">
         <v>1070</v>
       </c>
-      <c r="B72" s="2" t="s">
-        <v>1174</v>
+      <c r="B72" t="s">
+        <v>1170</v>
       </c>
       <c r="C72" t="s">
         <v>67</v>
@@ -7647,8 +7641,8 @@
       <c r="A73" s="10" t="s">
         <v>1071</v>
       </c>
-      <c r="B73" s="2" t="s">
-        <v>1175</v>
+      <c r="B73" t="s">
+        <v>1174</v>
       </c>
       <c r="C73" t="s">
         <v>68</v>
@@ -7678,12 +7672,12 @@
         <v>858</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="10" t="s">
         <v>1072</v>
       </c>
-      <c r="B74" s="2" t="s">
-        <v>1176</v>
+      <c r="B74" s="1" t="s">
+        <v>1175</v>
       </c>
       <c r="C74" t="s">
         <v>69</v>
@@ -7718,7 +7712,7 @@
         <v>1073</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="C75" t="s">
         <v>70</v>
@@ -7753,7 +7747,7 @@
         <v>1074</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="C76" t="s">
         <v>71</v>
@@ -7783,12 +7777,12 @@
         <v>861</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="10" t="s">
         <v>1075</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C77" t="s">
         <v>72</v>
@@ -7818,12 +7812,12 @@
         <v>862</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="10" t="s">
         <v>1076</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="C78" t="s">
         <v>73</v>
@@ -7858,7 +7852,7 @@
         <v>1077</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="C79" t="s">
         <v>74</v>
@@ -7893,7 +7887,7 @@
         <v>1078</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="C80" t="s">
         <v>75</v>
@@ -7928,7 +7922,7 @@
         <v>1079</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="C81" t="s">
         <v>76</v>
@@ -7963,7 +7957,7 @@
         <v>1080</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="C82" t="s">
         <v>77</v>
@@ -7998,7 +7992,7 @@
         <v>1081</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="C83" t="s">
         <v>78</v>
@@ -8033,7 +8027,7 @@
         <v>1082</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="C84" t="s">
         <v>79</v>
@@ -8068,7 +8062,7 @@
         <v>1083</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="C85" t="s">
         <v>80</v>
@@ -8103,7 +8097,7 @@
         <v>1084</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="C86" t="s">
         <v>81</v>
@@ -8138,7 +8132,7 @@
         <v>1085</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="C87" t="s">
         <v>82</v>
@@ -8173,7 +8167,7 @@
         <v>1086</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="C88" t="s">
         <v>83</v>
@@ -8208,7 +8202,7 @@
         <v>1087</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="C89" t="s">
         <v>84</v>
@@ -8238,12 +8232,12 @@
         <v>874</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="10" t="s">
         <v>1088</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="C90" t="s">
         <v>85</v>
@@ -8278,7 +8272,7 @@
         <v>1089</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="C91" t="s">
         <v>86</v>
@@ -8313,7 +8307,7 @@
         <v>1090</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="C92" t="s">
         <v>87</v>
@@ -8348,7 +8342,7 @@
         <v>1091</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="C93" t="s">
         <v>88</v>
@@ -8383,7 +8377,7 @@
         <v>1092</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="C94" t="s">
         <v>89</v>
@@ -8418,7 +8412,7 @@
         <v>1093</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="C95" t="s">
         <v>90</v>
@@ -8453,7 +8447,7 @@
         <v>1094</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="C96" t="s">
         <v>91</v>
@@ -8488,7 +8482,7 @@
         <v>92</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="C97" t="s">
         <v>92</v>
@@ -8523,7 +8517,7 @@
         <v>93</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="C98" t="s">
         <v>93</v>
@@ -8558,7 +8552,7 @@
         <v>94</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="C99" t="s">
         <v>94</v>
@@ -8592,8 +8586,8 @@
       <c r="A100" s="10" t="s">
         <v>1095</v>
       </c>
-      <c r="B100" s="2" t="s">
-        <v>1202</v>
+      <c r="B100" s="1" t="s">
+        <v>1201</v>
       </c>
       <c r="C100" t="s">
         <v>95</v>
@@ -8628,7 +8622,7 @@
         <v>96</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>1203</v>
+        <v>96</v>
       </c>
       <c r="C101" t="s">
         <v>96</v>
@@ -8663,7 +8657,7 @@
         <v>97</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>96</v>
+        <v>1202</v>
       </c>
       <c r="C102" t="s">
         <v>97</v>
@@ -8698,7 +8692,7 @@
         <v>98</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="C103" t="s">
         <v>98</v>
@@ -8733,7 +8727,7 @@
         <v>1096</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="C104" t="s">
         <v>99</v>
@@ -8763,12 +8757,12 @@
         <v>887</v>
       </c>
     </row>
-    <row r="105" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="10" t="s">
         <v>1097</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="C105" t="s">
         <v>100</v>
@@ -8803,7 +8797,7 @@
         <v>101</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>1207</v>
+        <v>101</v>
       </c>
       <c r="C106" t="s">
         <v>101</v>
@@ -8838,7 +8832,7 @@
         <v>1098</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>101</v>
+        <v>1138</v>
       </c>
       <c r="C107" t="s">
         <v>102</v>
@@ -8873,7 +8867,7 @@
         <v>1099</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>1138</v>
+        <v>1206</v>
       </c>
       <c r="C108" t="s">
         <v>103</v>
@@ -8908,7 +8902,7 @@
         <v>1100</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>1208</v>
+        <v>222</v>
       </c>
       <c r="C109" t="s">
         <v>104</v>
@@ -8943,7 +8937,7 @@
         <v>1101</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>222</v>
+        <v>1207</v>
       </c>
       <c r="C110" t="s">
         <v>105</v>
@@ -8978,7 +8972,7 @@
         <v>1102</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="C111" t="s">
         <v>106</v>
@@ -9013,7 +9007,7 @@
         <v>1103</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="C112" t="s">
         <v>107</v>
@@ -9048,7 +9042,7 @@
         <v>1104</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="C113" t="s">
         <v>108</v>
@@ -9083,7 +9077,7 @@
         <v>1105</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="C114" t="s">
         <v>109</v>
@@ -9118,7 +9112,7 @@
         <v>1106</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>1213</v>
+        <v>454</v>
       </c>
       <c r="C115" t="s">
         <v>110</v>
@@ -9153,7 +9147,7 @@
         <v>111</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>454</v>
+        <v>1196</v>
       </c>
       <c r="C116" t="s">
         <v>111</v>
@@ -9188,7 +9182,7 @@
         <v>1107</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>1198</v>
+        <v>1212</v>
       </c>
       <c r="C117" t="s">
         <v>112</v>
@@ -9223,7 +9217,7 @@
         <v>1108</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="C118" t="s">
         <v>113</v>
@@ -9258,7 +9252,7 @@
         <v>114</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>1215</v>
+        <v>114</v>
       </c>
       <c r="C119" t="s">
         <v>114</v>
@@ -9293,7 +9287,7 @@
         <v>115</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>114</v>
+        <v>232</v>
       </c>
       <c r="C120" t="s">
         <v>115</v>

</xml_diff>